<commit_message>
Fixed bug that would copy empty columns to the course equiv GUI
</commit_message>
<xml_diff>
--- a/team_project/src/course_equiv/course_equivalency_list.xlsx
+++ b/team_project/src/course_equiv/course_equivalency_list.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>CHEM1982</t>
   </si>
@@ -404,7 +404,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F3"/>
+  <dimension ref="C1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
@@ -416,9 +416,6 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
@@ -431,11 +428,11 @@
       <c r="F1" t="s">
         <v>3</v>
       </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
@@ -447,6 +444,9 @@
       </c>
       <c r="F2" t="s">
         <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>